<commit_message>
Updated Selenium Version and did necessary changes
</commit_message>
<xml_diff>
--- a/ELF_Base_Framework/src/test/resources/testData/testData.xlsx
+++ b/ELF_Base_Framework/src/test/resources/testData/testData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="64">
   <si>
     <t>no</t>
   </si>
@@ -124,13 +125,100 @@
   </si>
   <si>
     <t>dummy</t>
+  </si>
+  <si>
+    <t>Prady</t>
+  </si>
+  <si>
+    <t>Sumanth</t>
+  </si>
+  <si>
+    <t>Vikas</t>
+  </si>
+  <si>
+    <t>Chinni</t>
+  </si>
+  <si>
+    <t>Rakesh</t>
+  </si>
+  <si>
+    <t>Teju</t>
+  </si>
+  <si>
+    <t>Aani</t>
+  </si>
+  <si>
+    <t>Appu CM</t>
+  </si>
+  <si>
+    <t>Chinmaye</t>
+  </si>
+  <si>
+    <t>Sujatha</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Resort</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Ossur Lunch</t>
+  </si>
+  <si>
+    <t>Trek</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Snacks</t>
+  </si>
+  <si>
+    <t>500 + 100</t>
+  </si>
+  <si>
+    <t>Tips</t>
+  </si>
+  <si>
+    <t>Divide by 9</t>
+  </si>
+  <si>
+    <t>Overall Expenses</t>
+  </si>
+  <si>
+    <t>Trip Advance</t>
+  </si>
+  <si>
+    <t>Individual Expenses</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Divide by 10</t>
+  </si>
+  <si>
+    <t>Individual cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1120 + 280 + 80 + 170 </t>
+  </si>
+  <si>
+    <t>(27000/9 + 23240/10)</t>
+  </si>
+  <si>
+    <t>28296 - 250</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,21 +234,380 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="26">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -168,9 +615,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -454,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,4 +1449,419 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="23"/>
+      <c r="C3" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="6">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="6">
+        <v>850</v>
+      </c>
+      <c r="E4" s="6">
+        <v>170</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2000</v>
+      </c>
+      <c r="G4" s="6">
+        <v>300</v>
+      </c>
+      <c r="H4" s="25">
+        <v>20300</v>
+      </c>
+      <c r="I4" s="30">
+        <f>SUM(C4:H4)</f>
+        <v>33620</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="5">
+        <v>27000</v>
+      </c>
+      <c r="N4" s="11">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>4195</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1120</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="31">
+        <f>SUM(C5:H5)</f>
+        <v>5315</v>
+      </c>
+      <c r="J5" s="28">
+        <f>SUM(I5-5324)</f>
+        <v>-9</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="5">
+        <v>3300</v>
+      </c>
+      <c r="N5" s="11">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>280</v>
+      </c>
+      <c r="E6" s="2">
+        <v>80</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="31">
+        <f>SUM(C6:H6)</f>
+        <v>360</v>
+      </c>
+      <c r="J6" s="28">
+        <f>SUM(I6-5324)</f>
+        <v>-4964</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="4">
+        <v>500</v>
+      </c>
+      <c r="N6" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="31">
+        <f>SUM(C7:H7)</f>
+        <v>3000</v>
+      </c>
+      <c r="J7" s="28">
+        <f>SUM(I7-5324)</f>
+        <v>-2324</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="4">
+        <v>14340</v>
+      </c>
+      <c r="N7" s="13">
+        <v>14340</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="31">
+        <f>SUM(C8:H8)</f>
+        <v>2000</v>
+      </c>
+      <c r="J8" s="28">
+        <f>SUM(I8-5324)</f>
+        <v>-3324</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="4">
+        <v>2000</v>
+      </c>
+      <c r="N8" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D9" s="2">
+        <v>200</v>
+      </c>
+      <c r="E9" s="2">
+        <v>500</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="31">
+        <f>SUM(C9:H9)</f>
+        <v>3700</v>
+      </c>
+      <c r="J9" s="28">
+        <f>SUM(I9-5324)</f>
+        <v>-1624</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="13">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="2">
+        <v>100</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="31">
+        <f>SUM(C10:H10)</f>
+        <v>1100</v>
+      </c>
+      <c r="J10" s="28">
+        <f>SUM(I10-2324)</f>
+        <v>-1224</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" s="4">
+        <v>850</v>
+      </c>
+      <c r="N10" s="13">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="31">
+        <f>SUM(C11:H11)</f>
+        <v>3000</v>
+      </c>
+      <c r="J11" s="28">
+        <f>SUM(I11-5324)</f>
+        <v>-2324</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" s="18">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="31">
+        <f>SUM(C12:H12)</f>
+        <v>3000</v>
+      </c>
+      <c r="J12" s="28">
+        <f>SUM(I12-5324)</f>
+        <v>-2324</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="34"/>
+      <c r="N12" s="20">
+        <f>SUM(N4:N11)</f>
+        <v>50240</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2000</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="32">
+        <f>SUM(C13:H13)</f>
+        <v>2000</v>
+      </c>
+      <c r="J13" s="29">
+        <f>SUM(I13-5324)</f>
+        <v>-3324</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="2">
+        <v>27000</v>
+      </c>
+      <c r="O14" s="35">
+        <f>SUM(N14:N15)</f>
+        <v>50240</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" s="2">
+        <f>SUM(N5:N11)</f>
+        <v>23240</v>
+      </c>
+      <c r="O15" s="35"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f>SUM(J5:J13)</f>
+        <v>-21441</v>
+      </c>
+    </row>
+    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>6300</v>
+      </c>
+      <c r="M17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N17" s="3">
+        <v>5324</v>
+      </c>
+      <c r="O17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" s="3">
+        <v>2324</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="L3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>